<commit_message>
update BLDE, WLOU DSC/Gauge history
</commit_message>
<xml_diff>
--- a/hydrologicControls/NEON_AQU_Gauge_DSC_History.xlsx
+++ b/hydrologicControls/NEON_AQU_Gauge_DSC_History.xlsx
@@ -9,35 +9,34 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16500" tabRatio="704" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WLOU" sheetId="15" r:id="rId1"/>
     <sheet name="BLDE" sheetId="14" r:id="rId2"/>
     <sheet name="HOPB" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet28" sheetId="28" r:id="rId4"/>
-    <sheet name="LEWI" sheetId="3" r:id="rId5"/>
-    <sheet name="POSE" sheetId="2" r:id="rId6"/>
-    <sheet name="CUPE" sheetId="4" r:id="rId7"/>
-    <sheet name="GUIL" sheetId="5" r:id="rId8"/>
-    <sheet name="KING" sheetId="6" r:id="rId9"/>
-    <sheet name="MCDI" sheetId="7" r:id="rId10"/>
-    <sheet name="LECO" sheetId="8" r:id="rId11"/>
-    <sheet name="WALK" sheetId="9" r:id="rId12"/>
-    <sheet name="ARIK" sheetId="10" r:id="rId13"/>
-    <sheet name="BLUE" sheetId="12" r:id="rId14"/>
-    <sheet name="PRIN" sheetId="13" r:id="rId15"/>
-    <sheet name="COMO" sheetId="11" r:id="rId16"/>
-    <sheet name="SYCA" sheetId="16" r:id="rId17"/>
-    <sheet name="REDB" sheetId="17" r:id="rId18"/>
-    <sheet name="MCRA" sheetId="18" r:id="rId19"/>
-    <sheet name="MART" sheetId="19" r:id="rId20"/>
-    <sheet name="BIGC" sheetId="20" r:id="rId21"/>
-    <sheet name="TECR" sheetId="21" r:id="rId22"/>
-    <sheet name="CARI" sheetId="22" r:id="rId23"/>
-    <sheet name="OKSR" sheetId="23" r:id="rId24"/>
-    <sheet name="TOOK-IN" sheetId="24" r:id="rId25"/>
-    <sheet name="TOOK-OUT" sheetId="25" r:id="rId26"/>
+    <sheet name="LEWI" sheetId="3" r:id="rId4"/>
+    <sheet name="POSE" sheetId="2" r:id="rId5"/>
+    <sheet name="CUPE" sheetId="4" r:id="rId6"/>
+    <sheet name="GUIL" sheetId="5" r:id="rId7"/>
+    <sheet name="KING" sheetId="6" r:id="rId8"/>
+    <sheet name="MCDI" sheetId="7" r:id="rId9"/>
+    <sheet name="LECO" sheetId="8" r:id="rId10"/>
+    <sheet name="WALK" sheetId="9" r:id="rId11"/>
+    <sheet name="ARIK" sheetId="10" r:id="rId12"/>
+    <sheet name="BLUE" sheetId="12" r:id="rId13"/>
+    <sheet name="PRIN" sheetId="13" r:id="rId14"/>
+    <sheet name="COMO" sheetId="11" r:id="rId15"/>
+    <sheet name="SYCA" sheetId="16" r:id="rId16"/>
+    <sheet name="REDB" sheetId="17" r:id="rId17"/>
+    <sheet name="MCRA" sheetId="18" r:id="rId18"/>
+    <sheet name="MART" sheetId="19" r:id="rId19"/>
+    <sheet name="BIGC" sheetId="20" r:id="rId20"/>
+    <sheet name="TECR" sheetId="21" r:id="rId21"/>
+    <sheet name="CARI" sheetId="22" r:id="rId22"/>
+    <sheet name="OKSR" sheetId="23" r:id="rId23"/>
+    <sheet name="TOOK-IN" sheetId="24" r:id="rId24"/>
+    <sheet name="TOOK-OUT" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
   <si>
     <t>Gauge #</t>
   </si>
@@ -81,39 +80,18 @@
     <t>permanent</t>
   </si>
   <si>
-    <t>permanent?</t>
-  </si>
-  <si>
     <t>DSC1</t>
   </si>
   <si>
-    <t>DSC1?</t>
-  </si>
-  <si>
     <t>DSC2</t>
   </si>
   <si>
     <t>current gauge</t>
   </si>
   <si>
-    <t>at S1; gaugings from the beginning of the measurement record to 6/8/2017 should be associated with Gauge1 and DSC1.</t>
-  </si>
-  <si>
-    <t>at S1; gaugings from 6/8/2017 to 4/2/2019 are associated with Gauge2 and DSC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">at S2; gaugings from 4/3/19 to present are associated with Gauge3 and DSC2.  </t>
-  </si>
-  <si>
     <t>DSC XS Data?</t>
   </si>
   <si>
-    <t>Yes - 20170921, gauge surveyed</t>
-  </si>
-  <si>
-    <t>Yes - 20191126, gauge surveyed</t>
-  </si>
-  <si>
     <t>Continuous Gauge Location?</t>
   </si>
   <si>
@@ -130,6 +108,33 @@
   </si>
   <si>
     <t>There has been one DSC XS at WLOU and two staff gauges (permanent &amp; temporary).  The named location data should contain an offset between temporary and permanent and we have survey data to delineate the hydrologic controls at the discharge XS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first DSC measurement associated with the permanent gauge was on 8/7/18.  NLDB should contain continuous relationship from temporary gauge. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">not sure if this gauge is still installed.  </t>
+  </si>
+  <si>
+    <t>Yes - 20170921</t>
+  </si>
+  <si>
+    <t>Yes - 20191126</t>
+  </si>
+  <si>
+    <t>not sure if NLDB can relate Gauge1 to Gauge2</t>
+  </si>
+  <si>
+    <t>not sure if NLDB can relate Gauge2 to Gauge3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSC1 was located at S1; gaugings from 6/8/2017 to 4/2/2019 are associated with Gauge2 and DSC1.  The L0 stage/Q data lines up pretty well in this range.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSC2 is located at S2; gaugings from 4/3/19 to present are associated with Gauge3 and DSC2.  The L0 stage/Q data lines up pretty well in this range.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSC1 was located at S1; gaugings associated with Gauge1 and DSC1 go from 2016 (beginning of the measurement record) to 6/8/2017.  There is some scatter in the 2016 gaugings in relation to the 2017 ones.  </t>
   </si>
 </sst>
 </file>
@@ -197,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +221,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,10 +545,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>6</v>
@@ -551,25 +562,25 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>2016</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -580,22 +591,271 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="7">
         <v>43739</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S45" sqref="S45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U44" sqref="U44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="134" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2018</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43326</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8">
+        <v>43319</v>
+      </c>
+      <c r="E3" s="8">
+        <v>43326</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -603,166 +863,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +882,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +896,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+      <selection activeCell="V49" sqref="V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +924,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V49" sqref="V49"/>
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,20 +934,6 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -871,9 +963,9 @@
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="109.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="187.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -895,95 +987,98 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2016</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43419</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
-        <v>43419</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>42894</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>43419</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
+      <c r="F3" s="9">
+        <v>43466</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9">
+        <v>43525</v>
+      </c>
+      <c r="E4" s="8">
         <v>43696</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="1048576" spans="5:5" x14ac:dyDescent="0.25">
@@ -996,31 +1091,58 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1082,12 +1204,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1251,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated DSC XS history for COMO
</commit_message>
<xml_diff>
--- a/hydrologicControls/NEON_AQU_Gauge_DSC_History.xlsx
+++ b/hydrologicControls/NEON_AQU_Gauge_DSC_History.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8400" tabRatio="704" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8400" tabRatio="704" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WLOU_History" sheetId="15" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="42">
   <si>
     <t>Gauge #</t>
   </si>
@@ -134,15 +134,9 @@
     <t>Should be, check NLDB</t>
   </si>
   <si>
-    <t>The original discharge XS was located 3 meter downstream of S2 and the temporary staff gauge (Gauge1) in the tail of a pool.  DSC1 was never surveyed.</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>DSC2 is the current DSC XS, it is located 15-20 meters downstream of S2 and Gauge2 in a riffle so a different hydrologic unit as the Level TROLL and staff gauge…</t>
-  </si>
-  <si>
     <t>WY2015?</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>Gauge2 is the current gauge, DSC location has not changed over time; L1 edits are required for some gaugings (see L1Edits.csv).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSC1 is the original discharge XS, located 1 meter downstream of S2 and the temporary staff gauge (Gauge1) in the tail of a pool.  DSC1 was never surveyed but Gauge1 was during geomorphology.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSC2 is the current DSC XS, it is located 30 meters upstream of S2 and Gauge2 in a riffle so a different hydrologic unit as the Level TROLL and staff gauge.  DSC2 and Gauge2 were surveyed during geomorphology.  Hannah says it's possible that they began collecting DSC measurements at DSC2 before Gauge2 was installed in 2016.  Hannah thinks that the first measurement associated with DSC2 may have been 6/13/16.  </t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,6 +265,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,19 +607,19 @@
         <v>2016</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -635,19 +636,19 @@
         <v>43739</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +869,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -994,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -1049,7 +1050,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
@@ -1058,13 +1059,13 @@
         <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1081,19 +1082,19 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1105,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1177,7 @@
         <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1189,8 +1190,8 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3" s="9">
+        <v>42675</v>
       </c>
       <c r="E3" s="2">
         <v>43040</v>
@@ -1199,13 +1200,13 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PRIN 2019 discharge notes to DSC_XS_History spreadsheet
</commit_message>
<xml_diff>
--- a/hydrologicControls/NEON_AQU_Gauge_DSC_History.xlsx
+++ b/hydrologicControls/NEON_AQU_Gauge_DSC_History.xlsx
@@ -9,24 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8400" tabRatio="704" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8400" tabRatio="704" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="WLOU_History" sheetId="15" r:id="rId1"/>
     <sheet name="BLDE_History" sheetId="14" r:id="rId2"/>
     <sheet name="WALK_History" sheetId="9" r:id="rId3"/>
     <sheet name="COMO_History" sheetId="11" r:id="rId4"/>
-    <sheet name="HOPB" sheetId="1" r:id="rId5"/>
-    <sheet name="LEWI" sheetId="3" r:id="rId6"/>
-    <sheet name="POSE" sheetId="2" r:id="rId7"/>
-    <sheet name="CUPE" sheetId="4" r:id="rId8"/>
-    <sheet name="GUIL" sheetId="5" r:id="rId9"/>
-    <sheet name="KING" sheetId="6" r:id="rId10"/>
-    <sheet name="MCDI" sheetId="7" r:id="rId11"/>
-    <sheet name="LECO" sheetId="8" r:id="rId12"/>
-    <sheet name="ARIK" sheetId="10" r:id="rId13"/>
-    <sheet name="BLUE" sheetId="12" r:id="rId14"/>
-    <sheet name="PRIN" sheetId="13" r:id="rId15"/>
+    <sheet name="PRIN" sheetId="13" r:id="rId5"/>
+    <sheet name="HOPB" sheetId="1" r:id="rId6"/>
+    <sheet name="LEWI" sheetId="3" r:id="rId7"/>
+    <sheet name="POSE" sheetId="2" r:id="rId8"/>
+    <sheet name="CUPE" sheetId="4" r:id="rId9"/>
+    <sheet name="GUIL" sheetId="5" r:id="rId10"/>
+    <sheet name="KING" sheetId="6" r:id="rId11"/>
+    <sheet name="MCDI" sheetId="7" r:id="rId12"/>
+    <sheet name="LECO" sheetId="8" r:id="rId13"/>
+    <sheet name="ARIK" sheetId="10" r:id="rId14"/>
+    <sheet name="BLUE" sheetId="12" r:id="rId15"/>
     <sheet name="SYCA" sheetId="16" r:id="rId16"/>
     <sheet name="REDB" sheetId="17" r:id="rId17"/>
     <sheet name="MCRA" sheetId="18" r:id="rId18"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="44">
   <si>
     <t>Gauge #</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">DSC2 is the current DSC XS, it is located 30 meters upstream of S2 and Gauge2 in a riffle so a different hydrologic unit as the Level TROLL and staff gauge.  DSC2 and Gauge2 were surveyed during geomorphology.  Hannah says it's possible that they began collecting DSC measurements at DSC2 before Gauge2 was installed in 2016.  Hannah thinks that the first measurement associated with DSC2 may have been 6/13/16.  </t>
+  </si>
+  <si>
+    <t>PRIN 2019 note:</t>
+  </si>
+  <si>
+    <t>4 discharge bouts in 2019 were cancelled, see INC0036226 for details (only expect 21 for 2019).</t>
   </si>
 </sst>
 </file>
@@ -675,6 +681,20 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
@@ -684,7 +704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -698,7 +718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -712,26 +732,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M46" sqref="M46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1215,6 +1221,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -1356,7 +1387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1409,7 +1440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1471,7 +1502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1483,18 +1514,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>